<commit_message>
feat: add scripts etl to ods
</commit_message>
<xml_diff>
--- a/schema-build-draft.xlsx
+++ b/schema-build-draft.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\larruda\source\udacity\WeatherReviews\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77F2652C-B9F1-4FE2-8C46-18877F2328B5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABFEFFB4-4246-47C7-961F-EFC535E4AC8C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{99BDB2B9-A8DD-46B4-B4D1-20D9AAEB8FAC}"/>
+    <workbookView xWindow="3705" yWindow="2985" windowWidth="21600" windowHeight="11385" xr2:uid="{99BDB2B9-A8DD-46B4-B4D1-20D9AAEB8FAC}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Dictionary" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="151">
   <si>
     <t>yelp_business</t>
   </si>
@@ -485,6 +485,9 @@
   </si>
   <si>
     <t>2012-10-16</t>
+  </si>
+  <si>
+    <t>quarter</t>
   </si>
 </sst>
 </file>
@@ -671,15 +674,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -695,9 +692,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -740,6 +734,15 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1054,10 +1057,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E7DC5D9-9D3A-40E3-94C7-A89A2BFCA3D4}">
-  <dimension ref="B1:E138"/>
+  <dimension ref="B1:E139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="I129" sqref="I129"/>
+    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="E137" sqref="E137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1070,629 +1073,629 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="7" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="9"/>
-      <c r="C3" s="10" t="s">
+      <c r="B3" s="34"/>
+      <c r="C3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="10" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="9"/>
-      <c r="C4" s="10" t="s">
+      <c r="B4" s="34"/>
+      <c r="C4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="10" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="9"/>
-      <c r="C5" s="10" t="s">
+      <c r="B5" s="34"/>
+      <c r="C5" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="10" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="9"/>
-      <c r="C6" s="10" t="s">
+      <c r="B6" s="34"/>
+      <c r="C6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="10" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="9"/>
-      <c r="C7" s="10" t="s">
+      <c r="B7" s="34"/>
+      <c r="C7" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="10" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="9"/>
-      <c r="C8" s="10" t="s">
+      <c r="B8" s="34"/>
+      <c r="C8" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D8" s="13">
+      <c r="D8" s="11">
         <v>97218</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="10" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="9"/>
-      <c r="C9" s="10" t="s">
+      <c r="B9" s="34"/>
+      <c r="C9" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="D9" s="13">
+      <c r="D9" s="11">
         <v>45.588905898999997</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="10" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="9"/>
-      <c r="C10" s="10" t="s">
+      <c r="B10" s="34"/>
+      <c r="C10" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="D10" s="13">
+      <c r="D10" s="11">
         <v>-122.593330751</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="E10" s="10" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="9"/>
-      <c r="C11" s="10" t="s">
+      <c r="B11" s="34"/>
+      <c r="C11" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="D11" s="14">
+      <c r="D11" s="12">
         <v>4</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="E11" s="10" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="9"/>
-      <c r="C12" s="10" t="s">
+      <c r="B12" s="34"/>
+      <c r="C12" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="D12" s="13">
+      <c r="D12" s="11">
         <v>126</v>
       </c>
-      <c r="E12" s="12" t="s">
+      <c r="E12" s="10" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="9"/>
-      <c r="C13" s="10" t="s">
+      <c r="B13" s="34"/>
+      <c r="C13" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D13" s="13">
+      <c r="D13" s="11">
         <v>1</v>
       </c>
-      <c r="E13" s="12" t="s">
+      <c r="E13" s="10" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="9"/>
-      <c r="C14" s="10" t="s">
+      <c r="B14" s="34"/>
+      <c r="C14" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="E14" s="12" t="s">
+      <c r="E14" s="10" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="9"/>
-      <c r="C15" s="10" t="s">
+      <c r="B15" s="34"/>
+      <c r="C15" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="D15" s="13" t="b">
+      <c r="D15" s="11" t="b">
         <v>0</v>
       </c>
-      <c r="E15" s="12" t="s">
+      <c r="E15" s="10" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="9"/>
-      <c r="C16" s="10" t="s">
+      <c r="B16" s="34"/>
+      <c r="C16" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="15" t="s">
+      <c r="D16" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="E16" s="12" t="s">
+      <c r="E16" s="10" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="9"/>
-      <c r="C17" s="10" t="s">
+      <c r="B17" s="34"/>
+      <c r="C17" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="D17" s="13" t="b">
+      <c r="D17" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="E17" s="12" t="s">
+      <c r="E17" s="10" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="9"/>
-      <c r="C18" s="10" t="s">
+      <c r="B18" s="34"/>
+      <c r="C18" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D18" s="13" t="s">
+      <c r="D18" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="E18" s="12" t="s">
+      <c r="E18" s="10" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="9"/>
-      <c r="C19" s="10" t="s">
+      <c r="B19" s="34"/>
+      <c r="C19" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D19" s="13" t="b">
+      <c r="D19" s="11" t="b">
         <v>0</v>
       </c>
-      <c r="E19" s="12" t="s">
+      <c r="E19" s="10" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="9"/>
-      <c r="C20" s="10" t="s">
+      <c r="B20" s="34"/>
+      <c r="C20" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="D20" s="13" t="b">
+      <c r="D20" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="E20" s="12" t="s">
+      <c r="E20" s="10" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="9"/>
-      <c r="C21" s="10" t="s">
+      <c r="B21" s="34"/>
+      <c r="C21" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="D21" s="13" t="b">
+      <c r="D21" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="E21" s="12" t="s">
+      <c r="E21" s="10" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="9"/>
-      <c r="C22" s="10" t="s">
+      <c r="B22" s="34"/>
+      <c r="C22" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="D22" s="13" t="b">
+      <c r="D22" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="E22" s="12" t="s">
+      <c r="E22" s="10" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="9"/>
-      <c r="C23" s="10" t="s">
+      <c r="B23" s="34"/>
+      <c r="C23" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D23" s="13" t="s">
+      <c r="D23" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="E23" s="12" t="s">
+      <c r="E23" s="10" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="9"/>
-      <c r="C24" s="10" t="s">
+      <c r="B24" s="34"/>
+      <c r="C24" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="D24" s="13" t="b">
+      <c r="D24" s="11" t="b">
         <v>0</v>
       </c>
-      <c r="E24" s="12" t="s">
+      <c r="E24" s="10" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="9"/>
-      <c r="C25" s="10" t="s">
+      <c r="B25" s="34"/>
+      <c r="C25" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="D25" s="13" t="b">
+      <c r="D25" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="E25" s="12" t="s">
+      <c r="E25" s="10" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="9"/>
-      <c r="C26" s="10" t="s">
+      <c r="B26" s="34"/>
+      <c r="C26" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="D26" s="13">
+      <c r="D26" s="11">
         <v>2</v>
       </c>
-      <c r="E26" s="12" t="s">
+      <c r="E26" s="10" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B27" s="9"/>
-      <c r="C27" s="10" t="s">
+      <c r="B27" s="34"/>
+      <c r="C27" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D27" s="13" t="s">
+      <c r="D27" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="E27" s="12" t="s">
+      <c r="E27" s="10" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="9"/>
-      <c r="C28" s="10" t="s">
+      <c r="B28" s="34"/>
+      <c r="C28" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D28" s="13"/>
-      <c r="E28" s="12" t="s">
+      <c r="D28" s="11"/>
+      <c r="E28" s="10" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="9"/>
-      <c r="C29" s="10" t="s">
+      <c r="B29" s="34"/>
+      <c r="C29" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="D29" s="13"/>
-      <c r="E29" s="12" t="s">
+      <c r="D29" s="11"/>
+      <c r="E29" s="10" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="9"/>
-      <c r="C30" s="10" t="s">
+      <c r="B30" s="34"/>
+      <c r="C30" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="D30" s="13"/>
-      <c r="E30" s="12" t="s">
+      <c r="D30" s="11"/>
+      <c r="E30" s="10" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B31" s="9"/>
-      <c r="C31" s="10" t="s">
+      <c r="B31" s="34"/>
+      <c r="C31" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="D31" s="13"/>
-      <c r="E31" s="12" t="s">
+      <c r="D31" s="11"/>
+      <c r="E31" s="10" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B32" s="9"/>
-      <c r="C32" s="10" t="s">
+      <c r="B32" s="34"/>
+      <c r="C32" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D32" s="13"/>
-      <c r="E32" s="12" t="s">
+      <c r="D32" s="11"/>
+      <c r="E32" s="10" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B33" s="9"/>
-      <c r="C33" s="10" t="s">
+      <c r="B33" s="34"/>
+      <c r="C33" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="D33" s="13" t="b">
+      <c r="D33" s="11" t="b">
         <v>0</v>
       </c>
-      <c r="E33" s="12" t="s">
+      <c r="E33" s="10" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B34" s="9"/>
-      <c r="C34" s="10" t="s">
+      <c r="B34" s="34"/>
+      <c r="C34" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="D34" s="13" t="b">
+      <c r="D34" s="11" t="b">
         <v>0</v>
       </c>
-      <c r="E34" s="12" t="s">
+      <c r="E34" s="10" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B35" s="9"/>
-      <c r="C35" s="10" t="s">
+      <c r="B35" s="34"/>
+      <c r="C35" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="D35" s="13"/>
-      <c r="E35" s="12" t="s">
+      <c r="D35" s="11"/>
+      <c r="E35" s="10" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B36" s="9"/>
-      <c r="C36" s="10" t="s">
+      <c r="B36" s="34"/>
+      <c r="C36" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="D36" s="13"/>
-      <c r="E36" s="12" t="s">
+      <c r="D36" s="11"/>
+      <c r="E36" s="10" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B37" s="9"/>
-      <c r="C37" s="10" t="s">
+      <c r="B37" s="34"/>
+      <c r="C37" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D37" s="13" t="s">
+      <c r="D37" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="E37" s="12" t="s">
+      <c r="E37" s="10" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B38" s="9"/>
-      <c r="C38" s="10" t="s">
+      <c r="B38" s="34"/>
+      <c r="C38" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="D38" s="13"/>
-      <c r="E38" s="12" t="s">
+      <c r="D38" s="11"/>
+      <c r="E38" s="10" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B39" s="9"/>
-      <c r="C39" s="10" t="s">
+      <c r="B39" s="34"/>
+      <c r="C39" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D39" s="13" t="s">
+      <c r="D39" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="E39" s="12" t="s">
+      <c r="E39" s="10" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B40" s="9"/>
-      <c r="C40" s="10" t="s">
+      <c r="B40" s="34"/>
+      <c r="C40" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="D40" s="13"/>
-      <c r="E40" s="12" t="s">
+      <c r="D40" s="11"/>
+      <c r="E40" s="10" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B41" s="9"/>
-      <c r="C41" s="10" t="s">
+      <c r="B41" s="34"/>
+      <c r="C41" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="D41" s="13"/>
-      <c r="E41" s="12" t="s">
+      <c r="D41" s="11"/>
+      <c r="E41" s="10" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B42" s="9"/>
-      <c r="C42" s="10" t="s">
+      <c r="B42" s="34"/>
+      <c r="C42" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D42" s="13"/>
-      <c r="E42" s="12" t="s">
+      <c r="D42" s="11"/>
+      <c r="E42" s="10" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B43" s="9"/>
-      <c r="C43" s="10" t="s">
+      <c r="B43" s="34"/>
+      <c r="C43" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="D43" s="13"/>
-      <c r="E43" s="12" t="s">
+      <c r="D43" s="11"/>
+      <c r="E43" s="10" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B44" s="9"/>
-      <c r="C44" s="10" t="s">
+      <c r="B44" s="34"/>
+      <c r="C44" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="D44" s="13"/>
-      <c r="E44" s="12" t="s">
+      <c r="D44" s="11"/>
+      <c r="E44" s="10" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B45" s="9"/>
-      <c r="C45" s="10" t="s">
+      <c r="B45" s="34"/>
+      <c r="C45" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D45" s="13" t="s">
+      <c r="D45" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="E45" s="12" t="s">
+      <c r="E45" s="10" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B46" s="9"/>
-      <c r="C46" s="10" t="s">
+      <c r="B46" s="34"/>
+      <c r="C46" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D46" s="13" t="s">
+      <c r="D46" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="E46" s="12" t="s">
+      <c r="E46" s="10" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B47" s="9"/>
-      <c r="C47" s="10" t="s">
+      <c r="B47" s="34"/>
+      <c r="C47" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D47" s="13" t="s">
+      <c r="D47" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="E47" s="12" t="s">
+      <c r="E47" s="10" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B48" s="9"/>
-      <c r="C48" s="10" t="s">
+      <c r="B48" s="34"/>
+      <c r="C48" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D48" s="13" t="s">
+      <c r="D48" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="E48" s="12" t="s">
+      <c r="E48" s="10" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B49" s="9"/>
-      <c r="C49" s="10" t="s">
+      <c r="B49" s="34"/>
+      <c r="C49" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="D49" s="13" t="s">
+      <c r="D49" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="E49" s="12" t="s">
+      <c r="E49" s="10" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B50" s="9"/>
-      <c r="C50" s="10" t="s">
+      <c r="B50" s="34"/>
+      <c r="C50" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D50" s="13" t="s">
+      <c r="D50" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="E50" s="12" t="s">
+      <c r="E50" s="10" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B51" s="9"/>
-      <c r="C51" s="10" t="s">
+      <c r="B51" s="34"/>
+      <c r="C51" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D51" s="13" t="s">
+      <c r="D51" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="E51" s="12" t="s">
+      <c r="E51" s="10" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="52" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="16"/>
-      <c r="C52" s="17" t="s">
+      <c r="B52" s="35"/>
+      <c r="C52" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="D52" s="18" t="s">
+      <c r="D52" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="E52" s="19" t="s">
+      <c r="E52" s="16" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="54" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="55" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B55" s="5" t="s">
+      <c r="B55" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="C55" s="6" t="s">
+      <c r="C55" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="D55" s="7" t="s">
+      <c r="D55" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="E55" s="8" t="s">
+      <c r="E55" s="7" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B56" s="9"/>
-      <c r="C56" s="20" t="s">
+      <c r="B56" s="34"/>
+      <c r="C56" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D56" s="21" t="s">
+      <c r="D56" s="18" t="s">
         <v>123</v>
       </c>
-      <c r="E56" s="12" t="s">
+      <c r="E56" s="10" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="57" spans="2:5" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B57" s="16"/>
-      <c r="C57" s="22" t="s">
+      <c r="B57" s="35"/>
+      <c r="C57" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="D57" s="23" t="s">
+      <c r="D57" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="E57" s="19" t="s">
+      <c r="E57" s="16" t="s">
         <v>135</v>
       </c>
     </row>
@@ -1703,110 +1706,110 @@
       <c r="B59" s="1"/>
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B60" s="5" t="s">
+      <c r="B60" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="C60" s="6" t="s">
+      <c r="C60" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="D60" s="7" t="s">
+      <c r="D60" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="E60" s="8" t="s">
+      <c r="E60" s="7" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="61" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B61" s="9"/>
-      <c r="C61" s="20" t="s">
+      <c r="B61" s="34"/>
+      <c r="C61" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D61" s="21" t="s">
+      <c r="D61" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="E61" s="12" t="s">
+      <c r="E61" s="10" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="62" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B62" s="9"/>
-      <c r="C62" s="20" t="s">
+      <c r="B62" s="34"/>
+      <c r="C62" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="D62" s="13" t="b">
+      <c r="D62" s="11" t="b">
         <v>0</v>
       </c>
-      <c r="E62" s="12" t="s">
+      <c r="E62" s="10" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="63" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B63" s="9"/>
-      <c r="C63" s="20" t="s">
+      <c r="B63" s="34"/>
+      <c r="C63" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="D63" s="13"/>
-      <c r="E63" s="12" t="s">
+      <c r="D63" s="11"/>
+      <c r="E63" s="10" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="64" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B64" s="9"/>
-      <c r="C64" s="20" t="s">
+      <c r="B64" s="34"/>
+      <c r="C64" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="D64" s="13"/>
-      <c r="E64" s="12" t="s">
+      <c r="D64" s="11"/>
+      <c r="E64" s="10" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B65" s="9"/>
-      <c r="C65" s="20" t="s">
+      <c r="B65" s="34"/>
+      <c r="C65" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="D65" s="13"/>
-      <c r="E65" s="12" t="s">
+      <c r="D65" s="11"/>
+      <c r="E65" s="10" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="66" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B66" s="9"/>
-      <c r="C66" s="20" t="s">
+      <c r="B66" s="34"/>
+      <c r="C66" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="D66" s="13"/>
-      <c r="E66" s="12" t="s">
+      <c r="D66" s="11"/>
+      <c r="E66" s="10" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="67" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B67" s="9"/>
-      <c r="C67" s="20" t="s">
+      <c r="B67" s="34"/>
+      <c r="C67" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="D67" s="13"/>
-      <c r="E67" s="12" t="s">
+      <c r="D67" s="11"/>
+      <c r="E67" s="10" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="68" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B68" s="9"/>
-      <c r="C68" s="20" t="s">
+      <c r="B68" s="34"/>
+      <c r="C68" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="D68" s="13"/>
-      <c r="E68" s="12" t="s">
+      <c r="D68" s="11"/>
+      <c r="E68" s="10" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="69" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B69" s="16"/>
-      <c r="C69" s="24" t="s">
+      <c r="B69" s="35"/>
+      <c r="C69" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="D69" s="18"/>
-      <c r="E69" s="19" t="s">
+      <c r="D69" s="15"/>
+      <c r="E69" s="16" t="s">
         <v>136</v>
       </c>
     </row>
@@ -1817,124 +1820,124 @@
       <c r="B71" s="1"/>
     </row>
     <row r="72" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B72" s="5" t="s">
+      <c r="B72" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="C72" s="6" t="s">
+      <c r="C72" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="D72" s="7" t="s">
+      <c r="D72" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="E72" s="8" t="s">
+      <c r="E72" s="7" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="73" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B73" s="9"/>
-      <c r="C73" s="20" t="s">
+      <c r="B73" s="34"/>
+      <c r="C73" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="D73" s="21" t="s">
+      <c r="D73" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="E73" s="12" t="s">
+      <c r="E73" s="10" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="74" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B74" s="9"/>
-      <c r="C74" s="20" t="s">
+      <c r="B74" s="34"/>
+      <c r="C74" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D74" s="21" t="s">
+      <c r="D74" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="E74" s="12" t="s">
+      <c r="E74" s="10" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="75" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B75" s="9"/>
-      <c r="C75" s="20" t="s">
+      <c r="B75" s="34"/>
+      <c r="C75" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D75" s="21" t="s">
+      <c r="D75" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="E75" s="12" t="s">
+      <c r="E75" s="10" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="76" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B76" s="9"/>
-      <c r="C76" s="20" t="s">
+      <c r="B76" s="34"/>
+      <c r="C76" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="D76" s="13">
+      <c r="D76" s="11">
         <v>4</v>
       </c>
-      <c r="E76" s="12" t="s">
+      <c r="E76" s="10" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="77" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B77" s="9"/>
-      <c r="C77" s="20" t="s">
+      <c r="B77" s="34"/>
+      <c r="C77" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="D77" s="13">
+      <c r="D77" s="11">
         <v>4</v>
       </c>
-      <c r="E77" s="12" t="s">
+      <c r="E77" s="10" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="78" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B78" s="9"/>
-      <c r="C78" s="20" t="s">
+      <c r="B78" s="34"/>
+      <c r="C78" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="D78" s="13">
+      <c r="D78" s="11">
         <v>0</v>
       </c>
-      <c r="E78" s="12" t="s">
+      <c r="E78" s="10" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="79" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B79" s="9"/>
-      <c r="C79" s="20" t="s">
+      <c r="B79" s="34"/>
+      <c r="C79" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="D79" s="13">
+      <c r="D79" s="11">
         <v>2</v>
       </c>
-      <c r="E79" s="12" t="s">
+      <c r="E79" s="10" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="80" spans="2:5" ht="165" x14ac:dyDescent="0.25">
-      <c r="B80" s="9"/>
-      <c r="C80" s="25" t="s">
+      <c r="B80" s="34"/>
+      <c r="C80" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="D80" s="26" t="s">
+      <c r="D80" s="23" t="s">
         <v>121</v>
       </c>
-      <c r="E80" s="12" t="s">
+      <c r="E80" s="10" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="81" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B81" s="16"/>
-      <c r="C81" s="24" t="s">
+      <c r="B81" s="35"/>
+      <c r="C81" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="D81" s="27" t="s">
+      <c r="D81" s="24" t="s">
         <v>122</v>
       </c>
-      <c r="E81" s="19" t="s">
+      <c r="E81" s="16" t="s">
         <v>137</v>
       </c>
     </row>
@@ -1945,76 +1948,76 @@
       <c r="B83" s="1"/>
     </row>
     <row r="84" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B84" s="5" t="s">
+      <c r="B84" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="C84" s="6" t="s">
+      <c r="C84" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="D84" s="7" t="s">
+      <c r="D84" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="E84" s="8" t="s">
+      <c r="E84" s="7" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="85" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B85" s="9"/>
-      <c r="C85" s="20" t="s">
+      <c r="B85" s="34"/>
+      <c r="C85" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D85" s="21" t="s">
+      <c r="D85" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="E85" s="12" t="s">
+      <c r="E85" s="10" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="86" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B86" s="9"/>
-      <c r="C86" s="20" t="s">
+      <c r="B86" s="34"/>
+      <c r="C86" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D86" s="21" t="s">
+      <c r="D86" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="E86" s="12" t="s">
+      <c r="E86" s="10" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="87" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B87" s="9"/>
-      <c r="C87" s="20" t="s">
+      <c r="B87" s="34"/>
+      <c r="C87" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="D87" s="28" t="s">
+      <c r="D87" s="25" t="s">
         <v>128</v>
       </c>
-      <c r="E87" s="12" t="s">
+      <c r="E87" s="10" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="88" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B88" s="9"/>
-      <c r="C88" s="20" t="s">
+      <c r="B88" s="34"/>
+      <c r="C88" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="D88" s="28" t="s">
+      <c r="D88" s="25" t="s">
         <v>129</v>
       </c>
-      <c r="E88" s="12" t="s">
+      <c r="E88" s="10" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="89" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B89" s="16"/>
-      <c r="C89" s="24" t="s">
+      <c r="B89" s="35"/>
+      <c r="C89" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="D89" s="18">
+      <c r="D89" s="15">
         <v>0</v>
       </c>
-      <c r="E89" s="19" t="s">
+      <c r="E89" s="16" t="s">
         <v>138</v>
       </c>
     </row>
@@ -2025,278 +2028,278 @@
       <c r="B91" s="1"/>
     </row>
     <row r="92" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B92" s="5" t="s">
+      <c r="B92" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="C92" s="6" t="s">
+      <c r="C92" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="D92" s="7" t="s">
+      <c r="D92" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="E92" s="8" t="s">
+      <c r="E92" s="7" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="93" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B93" s="9"/>
-      <c r="C93" s="20" t="s">
+      <c r="B93" s="34"/>
+      <c r="C93" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D93" s="29" t="s">
+      <c r="D93" s="26" t="s">
         <v>113</v>
       </c>
-      <c r="E93" s="12" t="s">
+      <c r="E93" s="10" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="94" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B94" s="9"/>
-      <c r="C94" s="20" t="s">
+      <c r="B94" s="34"/>
+      <c r="C94" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="D94" s="21" t="s">
+      <c r="D94" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="E94" s="12" t="s">
+      <c r="E94" s="10" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="95" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B95" s="9"/>
-      <c r="C95" s="20" t="s">
+      <c r="B95" s="34"/>
+      <c r="C95" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="D95" s="13">
+      <c r="D95" s="11">
         <v>29</v>
       </c>
-      <c r="E95" s="12" t="s">
+      <c r="E95" s="10" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="96" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B96" s="9"/>
-      <c r="C96" s="20" t="s">
+      <c r="B96" s="34"/>
+      <c r="C96" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="D96" s="30" t="s">
+      <c r="D96" s="27" t="s">
         <v>115</v>
       </c>
-      <c r="E96" s="12" t="s">
+      <c r="E96" s="10" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="97" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B97" s="9"/>
-      <c r="C97" s="20" t="s">
+      <c r="B97" s="34"/>
+      <c r="C97" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="D97" s="13">
+      <c r="D97" s="11">
         <v>27</v>
       </c>
-      <c r="E97" s="12" t="s">
+      <c r="E97" s="10" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="98" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B98" s="9"/>
-      <c r="C98" s="20" t="s">
+      <c r="B98" s="34"/>
+      <c r="C98" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="D98" s="13">
+      <c r="D98" s="11">
         <v>1</v>
       </c>
-      <c r="E98" s="12" t="s">
+      <c r="E98" s="10" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="99" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B99" s="9"/>
-      <c r="C99" s="20" t="s">
+      <c r="B99" s="34"/>
+      <c r="C99" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="D99" s="13">
+      <c r="D99" s="11">
         <v>15</v>
       </c>
-      <c r="E99" s="12" t="s">
+      <c r="E99" s="10" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="100" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B100" s="9"/>
-      <c r="C100" s="20" t="s">
+      <c r="B100" s="34"/>
+      <c r="C100" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="D100" s="13"/>
-      <c r="E100" s="12" t="s">
+      <c r="D100" s="11"/>
+      <c r="E100" s="10" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="101" spans="2:5" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B101" s="9"/>
-      <c r="C101" s="31" t="s">
+      <c r="B101" s="34"/>
+      <c r="C101" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="D101" s="15" t="s">
+      <c r="D101" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="E101" s="12" t="s">
+      <c r="E101" s="10" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="102" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B102" s="9"/>
-      <c r="C102" s="20" t="s">
+      <c r="B102" s="34"/>
+      <c r="C102" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="D102" s="13">
+      <c r="D102" s="11">
         <v>1</v>
       </c>
-      <c r="E102" s="12" t="s">
+      <c r="E102" s="10" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="103" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B103" s="9"/>
-      <c r="C103" s="20" t="s">
+      <c r="B103" s="34"/>
+      <c r="C103" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="D103" s="13">
+      <c r="D103" s="11">
         <v>4.7300000000000004</v>
       </c>
-      <c r="E103" s="12" t="s">
+      <c r="E103" s="10" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="104" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B104" s="9"/>
-      <c r="C104" s="20" t="s">
+      <c r="B104" s="34"/>
+      <c r="C104" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="D104" s="13">
+      <c r="D104" s="11">
         <v>0</v>
       </c>
-      <c r="E104" s="12" t="s">
+      <c r="E104" s="10" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="105" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B105" s="9"/>
-      <c r="C105" s="20" t="s">
+      <c r="B105" s="34"/>
+      <c r="C105" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="D105" s="13">
+      <c r="D105" s="11">
         <v>0</v>
       </c>
-      <c r="E105" s="12" t="s">
+      <c r="E105" s="10" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="106" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B106" s="9"/>
-      <c r="C106" s="20" t="s">
+      <c r="B106" s="34"/>
+      <c r="C106" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="D106" s="13">
+      <c r="D106" s="11">
         <v>0</v>
       </c>
-      <c r="E106" s="12" t="s">
+      <c r="E106" s="10" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="107" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B107" s="9"/>
-      <c r="C107" s="20" t="s">
+      <c r="B107" s="34"/>
+      <c r="C107" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="D107" s="13">
+      <c r="D107" s="11">
         <v>0</v>
       </c>
-      <c r="E107" s="12" t="s">
+      <c r="E107" s="10" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="108" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B108" s="9"/>
-      <c r="C108" s="20" t="s">
+      <c r="B108" s="34"/>
+      <c r="C108" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="D108" s="13">
+      <c r="D108" s="11">
         <v>0</v>
       </c>
-      <c r="E108" s="12" t="s">
+      <c r="E108" s="10" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="109" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B109" s="9"/>
-      <c r="C109" s="20" t="s">
+      <c r="B109" s="34"/>
+      <c r="C109" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="D109" s="13">
+      <c r="D109" s="11">
         <v>0</v>
       </c>
-      <c r="E109" s="12" t="s">
+      <c r="E109" s="10" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="110" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B110" s="9"/>
-      <c r="C110" s="20" t="s">
+      <c r="B110" s="34"/>
+      <c r="C110" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="D110" s="13">
+      <c r="D110" s="11">
         <v>0</v>
       </c>
-      <c r="E110" s="12" t="s">
+      <c r="E110" s="10" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="111" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B111" s="9"/>
-      <c r="C111" s="20" t="s">
+      <c r="B111" s="34"/>
+      <c r="C111" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="D111" s="13">
+      <c r="D111" s="11">
         <v>0</v>
       </c>
-      <c r="E111" s="12" t="s">
+      <c r="E111" s="10" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="112" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B112" s="9"/>
-      <c r="C112" s="20" t="s">
+      <c r="B112" s="34"/>
+      <c r="C112" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="D112" s="13">
+      <c r="D112" s="11">
         <v>0</v>
       </c>
-      <c r="E112" s="12" t="s">
+      <c r="E112" s="10" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="113" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B113" s="9"/>
-      <c r="C113" s="20" t="s">
+      <c r="B113" s="34"/>
+      <c r="C113" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="D113" s="13">
+      <c r="D113" s="11">
         <v>0</v>
       </c>
-      <c r="E113" s="12" t="s">
+      <c r="E113" s="10" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="114" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B114" s="16"/>
-      <c r="C114" s="24" t="s">
+      <c r="B114" s="35"/>
+      <c r="C114" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="D114" s="18">
+      <c r="D114" s="15">
         <v>0</v>
       </c>
-      <c r="E114" s="19" t="s">
+      <c r="E114" s="16" t="s">
         <v>139</v>
       </c>
     </row>
@@ -2307,52 +2310,52 @@
       <c r="B116" s="1"/>
     </row>
     <row r="117" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B117" s="5" t="s">
+      <c r="B117" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="C117" s="6" t="s">
+      <c r="C117" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="D117" s="7" t="s">
+      <c r="D117" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="E117" s="8" t="s">
+      <c r="E117" s="7" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="118" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B118" s="9"/>
-      <c r="C118" s="20" t="s">
+      <c r="B118" s="34"/>
+      <c r="C118" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="D118" s="28" t="s">
+      <c r="D118" s="25" t="s">
         <v>130</v>
       </c>
-      <c r="E118" s="12" t="s">
+      <c r="E118" s="10" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="119" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B119" s="9"/>
-      <c r="C119" s="20" t="s">
+      <c r="B119" s="34"/>
+      <c r="C119" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="D119" s="13">
+      <c r="D119" s="11">
         <v>2.79</v>
       </c>
-      <c r="E119" s="12" t="s">
+      <c r="E119" s="10" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="120" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B120" s="16"/>
-      <c r="C120" s="24" t="s">
+      <c r="B120" s="35"/>
+      <c r="C120" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="D120" s="18">
+      <c r="D120" s="15">
         <v>3.65</v>
       </c>
-      <c r="E120" s="19" t="s">
+      <c r="E120" s="16" t="s">
         <v>140</v>
       </c>
     </row>
@@ -2366,161 +2369,173 @@
       <c r="B123" s="1"/>
     </row>
     <row r="124" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B124" s="5" t="s">
+      <c r="B124" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="C124" s="6" t="s">
+      <c r="C124" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="D124" s="7" t="s">
+      <c r="D124" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="E124" s="8" t="s">
+      <c r="E124" s="7" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="125" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B125" s="9"/>
-      <c r="C125" s="20" t="s">
+      <c r="B125" s="34"/>
+      <c r="C125" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="D125" s="28" t="s">
+      <c r="D125" s="25" t="s">
         <v>131</v>
       </c>
-      <c r="E125" s="12" t="s">
+      <c r="E125" s="10" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="126" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B126" s="9"/>
-      <c r="C126" s="20" t="s">
+      <c r="B126" s="34"/>
+      <c r="C126" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="D126" s="13">
+      <c r="D126" s="11">
         <v>61</v>
       </c>
-      <c r="E126" s="12" t="s">
+      <c r="E126" s="10" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="127" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B127" s="9"/>
-      <c r="C127" s="20" t="s">
+      <c r="B127" s="34"/>
+      <c r="C127" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="D127" s="13">
+      <c r="D127" s="11">
         <v>105</v>
       </c>
-      <c r="E127" s="12" t="s">
+      <c r="E127" s="10" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="128" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B128" s="9"/>
-      <c r="C128" s="20" t="s">
+      <c r="B128" s="34"/>
+      <c r="C128" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="D128" s="13">
+      <c r="D128" s="11">
         <v>76.099999999999994</v>
       </c>
-      <c r="E128" s="12" t="s">
+      <c r="E128" s="10" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="129" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B129" s="16"/>
-      <c r="C129" s="24" t="s">
+      <c r="B129" s="35"/>
+      <c r="C129" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="D129" s="18">
+      <c r="D129" s="15">
         <v>98.7</v>
       </c>
-      <c r="E129" s="19" t="s">
+      <c r="E129" s="16" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="131" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="132" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B132" s="32"/>
-      <c r="C132" s="6" t="s">
+      <c r="B132" s="29"/>
+      <c r="C132" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="D132" s="7" t="s">
+      <c r="D132" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="E132" s="8" t="s">
+      <c r="E132" s="7" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="133" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B133" s="33"/>
-      <c r="C133" s="20" t="s">
+      <c r="B133" s="30"/>
+      <c r="C133" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="D133" s="28" t="s">
+      <c r="D133" s="25" t="s">
         <v>122</v>
       </c>
-      <c r="E133" s="12" t="s">
+      <c r="E133" s="10" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="134" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B134" s="33"/>
-      <c r="C134" s="20" t="s">
+      <c r="B134" s="30"/>
+      <c r="C134" s="17" t="s">
         <v>117</v>
       </c>
-      <c r="D134" s="34" t="s">
+      <c r="D134" s="31" t="s">
         <v>149</v>
       </c>
-      <c r="E134" s="12" t="s">
+      <c r="E134" s="10" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="135" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B135" s="33"/>
-      <c r="C135" s="20" t="s">
+      <c r="B135" s="30"/>
+      <c r="C135" s="17" t="s">
         <v>145</v>
       </c>
-      <c r="D135" s="13">
+      <c r="D135" s="11">
         <v>16</v>
       </c>
-      <c r="E135" s="12" t="s">
+      <c r="E135" s="10" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="136" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B136" s="33"/>
-      <c r="C136" s="20" t="s">
+      <c r="B136" s="30"/>
+      <c r="C136" s="17" t="s">
         <v>146</v>
       </c>
-      <c r="D136" s="13">
+      <c r="D136" s="11">
         <v>25</v>
       </c>
-      <c r="E136" s="12" t="s">
+      <c r="E136" s="10" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="137" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B137" s="33"/>
-      <c r="C137" s="20" t="s">
+      <c r="B137" s="30"/>
+      <c r="C137" s="17" t="s">
         <v>147</v>
       </c>
-      <c r="D137" s="13">
+      <c r="D137" s="11">
         <v>10</v>
       </c>
-      <c r="E137" s="12" t="s">
+      <c r="E137" s="10" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="138" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B138" s="35"/>
-      <c r="C138" s="24" t="s">
+    <row r="138" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B138" s="30"/>
+      <c r="C138" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="D138" s="11">
+        <v>4</v>
+      </c>
+      <c r="E138" s="10" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="139" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B139" s="32"/>
+      <c r="C139" s="21" t="s">
         <v>148</v>
       </c>
-      <c r="D138" s="18">
+      <c r="D139" s="15">
         <v>2012</v>
       </c>
-      <c r="E138" s="19" t="s">
+      <c r="E139" s="16" t="s">
         <v>144</v>
       </c>
     </row>

</xml_diff>